<commit_message>
go to inside link
</commit_message>
<xml_diff>
--- a/3080.xlsx
+++ b/3080.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E289"/>
+  <dimension ref="A1:F289"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,12 +446,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>rated out of 5</t>
+          <t>Rated out of 5</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>Number of reviews</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Link of the item</t>
         </is>
       </c>
     </row>
@@ -481,6 +486,11 @@
           <t>86</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -508,6 +518,11 @@
           <t>86</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -535,6 +550,11 @@
           <t>86</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -562,6 +582,11 @@
           <t>86</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -589,6 +614,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -616,6 +646,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -643,6 +678,11 @@
           <t>50</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -670,6 +710,11 @@
           <t>83</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -697,6 +742,11 @@
           <t>83</t>
         </is>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -724,6 +774,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -751,6 +806,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -778,6 +838,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -805,6 +870,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -832,6 +902,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -859,6 +934,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -886,6 +966,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -913,6 +998,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -940,6 +1030,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -967,6 +1062,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -994,6 +1094,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1021,6 +1126,11 @@
           <t>58</t>
         </is>
       </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1048,6 +1158,11 @@
           <t>129</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1075,6 +1190,11 @@
           <t>129</t>
         </is>
       </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1102,6 +1222,11 @@
           <t>129</t>
         </is>
       </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1129,6 +1254,11 @@
           <t>129</t>
         </is>
       </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1156,6 +1286,11 @@
           <t>129</t>
         </is>
       </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1183,6 +1318,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1210,6 +1350,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1237,6 +1382,11 @@
           <t>7</t>
         </is>
       </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1264,6 +1414,11 @@
           <t>7</t>
         </is>
       </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1291,6 +1446,11 @@
           <t>14</t>
         </is>
       </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1318,6 +1478,11 @@
           <t>14</t>
         </is>
       </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1345,6 +1510,11 @@
           <t>14</t>
         </is>
       </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1372,6 +1542,11 @@
           <t>14</t>
         </is>
       </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1399,6 +1574,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1426,6 +1606,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1453,6 +1638,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1480,6 +1670,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1507,6 +1702,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1534,6 +1734,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1561,6 +1766,11 @@
           <t>46</t>
         </is>
       </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1588,6 +1798,11 @@
           <t>46</t>
         </is>
       </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1615,6 +1830,11 @@
           <t>96</t>
         </is>
       </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1642,6 +1862,11 @@
           <t>96</t>
         </is>
       </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1669,6 +1894,11 @@
           <t>96</t>
         </is>
       </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1696,6 +1926,11 @@
           <t>96</t>
         </is>
       </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1723,6 +1958,11 @@
           <t>96</t>
         </is>
       </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1750,6 +1990,11 @@
           <t>96</t>
         </is>
       </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1777,6 +2022,11 @@
           <t>96</t>
         </is>
       </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1804,6 +2054,11 @@
           <t>112</t>
         </is>
       </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1831,6 +2086,11 @@
           <t>112</t>
         </is>
       </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1858,6 +2118,11 @@
           <t>112</t>
         </is>
       </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1885,6 +2150,11 @@
           <t>112</t>
         </is>
       </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1912,6 +2182,11 @@
           <t>112</t>
         </is>
       </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1939,6 +2214,11 @@
           <t>106</t>
         </is>
       </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1966,6 +2246,11 @@
           <t>106</t>
         </is>
       </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1993,6 +2278,11 @@
           <t>106</t>
         </is>
       </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2020,6 +2310,11 @@
           <t>106</t>
         </is>
       </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2047,6 +2342,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2074,6 +2374,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2101,6 +2406,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2128,6 +2438,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2155,6 +2470,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2182,6 +2502,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2209,6 +2534,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2236,6 +2566,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2263,6 +2598,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2290,6 +2630,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2317,6 +2662,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2344,6 +2694,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2371,6 +2726,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2398,6 +2758,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2425,6 +2790,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2452,6 +2822,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2479,6 +2854,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2506,6 +2886,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2533,6 +2918,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2560,6 +2950,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2587,6 +2982,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2614,6 +3014,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2641,6 +3046,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2668,6 +3078,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2695,6 +3110,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2722,6 +3142,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2749,6 +3174,11 @@
           <t>54</t>
         </is>
       </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2776,6 +3206,11 @@
           <t>8</t>
         </is>
       </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2803,6 +3238,11 @@
           <t>8</t>
         </is>
       </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2830,6 +3270,11 @@
           <t>8</t>
         </is>
       </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2857,6 +3302,11 @@
           <t>206</t>
         </is>
       </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2884,6 +3334,11 @@
           <t>206</t>
         </is>
       </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2911,6 +3366,11 @@
           <t>206</t>
         </is>
       </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2938,6 +3398,11 @@
           <t>206</t>
         </is>
       </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2965,6 +3430,11 @@
           <t>18</t>
         </is>
       </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -2992,6 +3462,11 @@
           <t>18</t>
         </is>
       </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3019,6 +3494,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3046,6 +3526,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3073,6 +3558,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3100,6 +3590,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3127,6 +3622,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3154,6 +3654,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3181,6 +3686,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3208,6 +3718,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3235,6 +3750,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3262,6 +3782,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3289,6 +3814,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3316,6 +3846,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -3343,6 +3878,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -3370,6 +3910,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -3397,6 +3942,11 @@
           <t>27</t>
         </is>
       </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -3424,6 +3974,11 @@
           <t>27</t>
         </is>
       </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -3451,6 +4006,11 @@
           <t>27</t>
         </is>
       </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -3478,6 +4038,11 @@
           <t>27</t>
         </is>
       </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -3505,6 +4070,11 @@
           <t>27</t>
         </is>
       </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -3532,6 +4102,11 @@
           <t>58</t>
         </is>
       </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -3559,6 +4134,11 @@
           <t>58</t>
         </is>
       </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -3586,6 +4166,11 @@
           <t>58</t>
         </is>
       </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -3613,6 +4198,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -3640,6 +4230,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -3667,6 +4262,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -3694,6 +4294,11 @@
           <t>112</t>
         </is>
       </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -3721,6 +4326,11 @@
           <t>112</t>
         </is>
       </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -3748,6 +4358,11 @@
           <t>9</t>
         </is>
       </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -3775,6 +4390,11 @@
           <t>9</t>
         </is>
       </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -3802,6 +4422,11 @@
           <t>9</t>
         </is>
       </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -3829,6 +4454,11 @@
           <t>9</t>
         </is>
       </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -3856,6 +4486,11 @@
           <t>9</t>
         </is>
       </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -3883,6 +4518,11 @@
           <t>9</t>
         </is>
       </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -3910,6 +4550,11 @@
           <t>19</t>
         </is>
       </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -3937,6 +4582,11 @@
           <t>19</t>
         </is>
       </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -3964,6 +4614,11 @@
           <t>19</t>
         </is>
       </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -3991,6 +4646,11 @@
           <t>19</t>
         </is>
       </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -4018,6 +4678,11 @@
           <t>19</t>
         </is>
       </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -4045,6 +4710,11 @@
           <t>19</t>
         </is>
       </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -4072,6 +4742,11 @@
           <t>19</t>
         </is>
       </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -4099,6 +4774,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -4126,6 +4806,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -4153,6 +4838,11 @@
           <t>15</t>
         </is>
       </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -4180,6 +4870,11 @@
           <t>15</t>
         </is>
       </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -4207,6 +4902,11 @@
           <t>15</t>
         </is>
       </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -4234,6 +4934,11 @@
           <t>15</t>
         </is>
       </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -4261,6 +4966,11 @@
           <t>15</t>
         </is>
       </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -4288,6 +4998,11 @@
           <t>15</t>
         </is>
       </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -4315,6 +5030,11 @@
           <t>35</t>
         </is>
       </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -4342,6 +5062,11 @@
           <t>35</t>
         </is>
       </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -4369,6 +5094,11 @@
           <t>35</t>
         </is>
       </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -4396,6 +5126,11 @@
           <t>35</t>
         </is>
       </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -4423,6 +5158,11 @@
           <t>13</t>
         </is>
       </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -4450,6 +5190,11 @@
           <t>13</t>
         </is>
       </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -4477,6 +5222,11 @@
           <t>173</t>
         </is>
       </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -4504,6 +5254,11 @@
           <t>173</t>
         </is>
       </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -4531,6 +5286,11 @@
           <t>89</t>
         </is>
       </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -4558,6 +5318,11 @@
           <t>89</t>
         </is>
       </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -4585,6 +5350,11 @@
           <t>68</t>
         </is>
       </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -4612,6 +5382,11 @@
           <t>15</t>
         </is>
       </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -4639,6 +5414,11 @@
           <t>15</t>
         </is>
       </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -4666,6 +5446,11 @@
           <t>15</t>
         </is>
       </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -4693,6 +5478,11 @@
           <t>15</t>
         </is>
       </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -4720,6 +5510,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -4747,6 +5542,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -4774,6 +5574,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -4801,6 +5606,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -4828,6 +5638,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -4855,6 +5670,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -4882,98 +5702,118 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
+          <t>ASUS ROG Strix GeForce RTX 3080 V2 OC Edition 10GB GDDR6X PCI Express 4.0 x16 Video Card ROG-STRIX-RTX3080-O10G-V2-GAMING (LHR)</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>$ 649</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Free Shipping</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>rated 3.3 out of 5</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>ROG-STRIX-RTX3080-O10G-V2-GAMING</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>$ 649</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Free Shipping</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>rated 3.3 out of 5</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
           <t>MSI Suprim GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 Video Card RTX 3080 SUPRIM X 10G 
 (LHR)</t>
         </is>
       </c>
-      <c r="B167" t="inlineStr">
+      <c r="B169" t="inlineStr">
         <is>
           <t>$ 678</t>
         </is>
       </c>
-      <c r="C167" t="inlineStr">
-        <is>
-          <t>Free Shipping</t>
-        </is>
-      </c>
-      <c r="D167" t="inlineStr">
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Free Shipping</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
         <is>
           <t>rated 5 out of 5</t>
         </is>
       </c>
-      <c r="E167" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>--RTX 3080 SUPRIM X 10G</t>
-        </is>
-      </c>
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>$ 678</t>
-        </is>
-      </c>
-      <c r="C168" t="inlineStr">
-        <is>
-          <t>Free Shipping</t>
-        </is>
-      </c>
-      <c r="D168" t="inlineStr">
-        <is>
-          <t>rated 5 out of 5</t>
-        </is>
-      </c>
-      <c r="E168" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>MSI Gaming GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 ATX Video Card RTX 3080 GAMING Z TRIO 10G LHR</t>
-        </is>
-      </c>
-      <c r="B169" t="inlineStr">
-        <is>
-          <t>$ 619</t>
-        </is>
-      </c>
-      <c r="C169" t="inlineStr">
-        <is>
-          <t>Free Shipping</t>
-        </is>
-      </c>
-      <c r="D169" t="inlineStr">
-        <is>
-          <t>rated 4 out of 5</t>
-        </is>
-      </c>
       <c r="E169" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>RTX 3080 GAMING Z TRIO 10G L</t>
+          <t>--RTX 3080 SUPRIM X 10G</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>$ 619</t>
+          <t>$ 678</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -4983,24 +5823,29 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>rated 4 out of 5</t>
+          <t>rated 5 out of 5</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>MSI Ventus GeForce RTX 3080 Ti 12GB GDDR6X PCI Express 4.0 ATX Video Card -RTX 3080 Ti Ventus 3X 12G OC--</t>
+          <t>MSI Gaming GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 ATX Video Card RTX 3080 GAMING Z TRIO 10G LHR</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>$ 799</t>
+          <t>$ 619</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -5016,18 +5861,23 @@
       <c r="E171" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>-RTX 3080 Ti Ventus 3X</t>
+          <t>RTX 3080 GAMING Z TRIO 10G L</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>$ 799</t>
+          <t>$ 619</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -5043,18 +5893,23 @@
       <c r="E172" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>ASUS ROG Strix GeForce RTX 3080 V2 OC Edition 10GB GDDR6X PCI Express 4.0 x16 Video Card ROG-STRIX-RTX3080-O10G-V2-GAMING (LHR)</t>
+          <t>MSI Ventus GeForce RTX 3080 Ti 12GB GDDR6X PCI Express 4.0 ATX Video Card -RTX 3080 Ti Ventus 3X 12G OC--</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>$ 649</t>
+          <t>$ 799</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -5070,18 +5925,23 @@
       <c r="E173" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>ROG-STRIX-RTX3080-O10G-V2-GAMING</t>
+          <t>-RTX 3080 Ti Ventus 3X</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>$ 649</t>
+          <t>$ 799</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -5097,6 +5957,11 @@
       <c r="E174" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
@@ -5126,6 +5991,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -5153,6 +6023,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -5180,6 +6055,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -5207,6 +6087,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -5234,6 +6119,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -5261,6 +6151,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -5288,6 +6183,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -5315,6 +6215,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -5342,6 +6247,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -5369,16 +6279,21 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>MSI Gaming GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 Video Card RTX 3080 GAMING X TRIO 10G</t>
+          <t>MSI RTX 3080 SUPRIM X 10G LHR Suprim GeForce RTX 3080 Video Card</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>$ 619</t>
+          <t>$ 678</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -5394,18 +6309,23 @@
       <c r="E185" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>RTX 3080 GAMING X TRIO 10</t>
+          <t>RTX3080SuprimX10GLHRSNRFB</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>$ 619</t>
+          <t>$ 678</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -5421,18 +6341,23 @@
       <c r="E186" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>MSI RTX 3080 SUPRIM X 10G LHR Suprim GeForce RTX 3080 Video Card</t>
+          <t>GIGABYTE Gaming OC GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 ATX Video Card GV-N3080GAMING OC-10GD (rev. 2.0) (LHR)</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>$ 678</t>
+          <t>$ 679</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -5448,18 +6373,23 @@
       <c r="E187" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>RTX3080SuprimX10GLHRSNRFB</t>
+          <t>GV-N3080GAMING OC-10GD REV</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>$ 678</t>
+          <t>$ 679</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -5475,23 +6405,28 @@
       <c r="E188" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>GIGABYTE Gaming OC GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 ATX Video Card GV-N3080GAMING OC-10GD (rev. 2.0) (LHR)</t>
+          <t>MSI GeForce RTX 3080 Suprim X 10G LHR 10GB GDRR6X 320-Bit HDMI/DP Graphics Card</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>$ 679</t>
+          <t>$ 699</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>Free Shipping</t>
+          <t>$7.00 Shipping</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
@@ -5502,23 +6437,28 @@
       <c r="E189" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>GV-N3080GAMING OC-10GD REV</t>
+          <t>RTX3080SUPRIMX10GLHR</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>$ 679</t>
+          <t>$ 699</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>Free Shipping</t>
+          <t>$7.00 Shipping</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
@@ -5529,23 +6469,28 @@
       <c r="E190" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>MSI GeForce RTX 3080 Suprim X 10G LHR 10GB GDRR6X 320-Bit HDMI/DP Graphics Card</t>
+          <t>GIGABYTE Gaming GeForce RTX 3080 Ti Video Card GV-N308TGAMING OC-12GD</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>$ 699</t>
+          <t>$ 959</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>$7.00 Shipping</t>
+          <t>Free Shipping</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
@@ -5556,23 +6501,28 @@
       <c r="E191" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>RTX3080SUPRIMX10GLHR</t>
+          <t>MSI Gaming GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 Video Card RTX 3080 GAMING X TRIO 10G</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>$ 699</t>
+          <t>$ 619</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>$7.00 Shipping</t>
+          <t>Free Shipping</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
@@ -5583,18 +6533,23 @@
       <c r="E192" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>GIGABYTE Gaming GeForce RTX 3080 Ti Video Card GV-N308TGAMING OC-12GD</t>
+          <t>RTX 3080 GAMING X TRIO 10</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>$ 959</t>
+          <t>$ 619</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -5610,6 +6565,11 @@
       <c r="E193" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
@@ -5639,6 +6599,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -5666,6 +6631,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -5693,6 +6663,11 @@
           <t>39</t>
         </is>
       </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -5720,16 +6695,21 @@
           <t>39</t>
         </is>
       </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>MSI RTX 3080 Ti Ventus 3X 12G OC Ventus GeForce RTX 3080 Ti Video Card</t>
+          <t>EVGA GeForce RTX 3080 XC3 ULTRA GAMING Video Card, 10G-P5-3885-KR, 10GB GDDR6X, iCX3 Cooling, ARGB LED, Metal Backplate</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>$ 799</t>
+          <t>$ 639</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -5739,19 +6719,24 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>rated 4.3 out of 5</t>
+          <t>rated 4 out of 5</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>3080tiVentus3X12GOCSNRFB</t>
+          <t>MSI RTX 3080 Ti Ventus 3X 12G OC Ventus GeForce RTX 3080 Ti Video Card</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -5766,24 +6751,29 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>rated 4.3 out of 5</t>
+          <t>rated 4 out of 5</t>
         </is>
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>EVGA GeForce RTX 3080 XC3 ULTRA GAMING Video Card, 10G-P5-3885-KR, 10GB GDDR6X, iCX3 Cooling, ARGB LED, Metal Backplate</t>
+          <t>3080tiVentus3X12GOCSNRFB</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>$ 639</t>
+          <t>$ 799</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -5799,6 +6789,11 @@
       <c r="E200" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
@@ -5828,6 +6823,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -5855,6 +6855,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -5882,6 +6887,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -5909,6 +6919,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -5936,6 +6951,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -5963,6 +6983,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -5990,6 +7015,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -6017,6 +7047,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -6044,6 +7079,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -6071,92 +7111,112 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>MSI Suprim GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 Video Card RTX 3080 SUPRIM 10G</t>
+          <t>ASUS ROG STRIX GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 x16 ATX Video Card ROG-STRIX-RTX3080-O10G-WHITE-V2 (LHR)</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>$ 699</t>
+          <t>$ 769</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>$20.00 Shipping</t>
+          <t>Free Shipping</t>
         </is>
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>rated 5 out of 5</t>
+          <t>rated 2 out of 5</t>
         </is>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>RTX 3080 SUPRIM 10G</t>
+          <t>RTX3080-O10G-WHT-V2SNRFB</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>$ 699</t>
+          <t>$ 769</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>$20.00 Shipping</t>
+          <t>Free Shipping</t>
         </is>
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>rated 5 out of 5</t>
+          <t>rated 2 out of 5</t>
         </is>
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>MSI Gaming GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 Video Card RTX 3080 GAMING X TRIO 10G</t>
+          <t>GIGABYTE GV-N308TGAMING OC-12GD Gaming GeForce RTX 3080 Ti Video Card</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>$ 699</t>
+          <t>$ 739</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>$20.00 Shipping</t>
+          <t>Free Shipping</t>
         </is>
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>rated 5 out of 5</t>
+          <t>rated 2 out of 5</t>
         </is>
       </c>
       <c r="E213" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>3080GamingXTrio10G</t>
+          <t>MSI Suprim GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 Video Card RTX 3080 SUPRIM 10G</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -6171,29 +7231,34 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>rated 5 out of 5</t>
+          <t>rated 2 out of 5</t>
         </is>
       </c>
       <c r="E214" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>ASUS ROG STRIX GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 x16 ATX Video Card ROG-STRIX-RTX3080-O10G-WHITE-V2 (LHR)</t>
+          <t>RTX 3080 SUPRIM 10G</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>$ 769</t>
+          <t>$ 699</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>Free Shipping</t>
+          <t>$20.00 Shipping</t>
         </is>
       </c>
       <c r="D215" t="inlineStr">
@@ -6203,24 +7268,29 @@
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>RTX3080-O10G-WHT-V2SNRFB</t>
+          <t>MSI Gaming GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 Video Card RTX 3080 GAMING X TRIO 10G</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>$ 769</t>
+          <t>$ 699</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>Free Shipping</t>
+          <t>$20.00 Shipping</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
@@ -6230,24 +7300,29 @@
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>GIGABYTE GV-N308TGAMING OC-12GD Gaming GeForce RTX 3080 Ti Video Card</t>
+          <t>3080GamingXTrio10G</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>$ 739</t>
+          <t>$ 699</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>Free Shipping</t>
+          <t>$20.00 Shipping</t>
         </is>
       </c>
       <c r="D217" t="inlineStr">
@@ -6258,18 +7333,23 @@
       <c r="E217" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>MSI RTX 3080 Ti SUPRIM X 12G Suprim GeForce RTX 3080 Ti Video Card</t>
+          <t>ASUS TUF Gaming NVIDIA GeForce RTX 3080 TUF-RTX3080-10G-GAMING Graphics Card with hub (Refurbished)</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>$ 799</t>
+          <t>$ 899</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
@@ -6285,13 +7365,18 @@
       <c r="E218" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>RTX3080TiSUPRIMX12GSNRFB</t>
+          <t>MSI RTX 3080 Ti SUPRIM X 12G Suprim GeForce RTX 3080 Ti Video Card</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
@@ -6312,18 +7397,23 @@
       <c r="E219" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>MSI GeForce RTX 3080 VENTUS 3X 10G 10GB GDDR6X Graphics Card - Black</t>
+          <t>RTX3080TiSUPRIMX12GSNRFB</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>$ 1,137</t>
+          <t>$ 799</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -6339,18 +7429,23 @@
       <c r="E220" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>RTX-3080-VENTUS-3X-10G</t>
+          <t>GIGABYTE GeForce RTX 3080 VISION OC 10GB Video Card, GV-N3080VISION OC-10GD (REV2.0)</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>$ 1,137</t>
+          <t>$ 639</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -6366,18 +7461,23 @@
       <c r="E221" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>ASUS TUF Gaming NVIDIA GeForce RTX 3080 TUF-RTX3080-10G-GAMING Graphics Card with hub (Refurbished)</t>
+          <t>GV-N3080VISIONOC-10GDREV2SNRFB</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>$ 899</t>
+          <t>$ 639</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -6393,18 +7493,23 @@
       <c r="E222" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>GIGABYTE 3080 Graphics card AORUS GIGABYTE GeForce RTX 3080 MASTER 10GB PCI Express 4.0 ATX Video Card (rev. 3.0) GV-N3080AORUS M-10GD (LHR)</t>
+          <t>ASUS TUF Gaming NVIDIA GeForce RTX 3080 Graphics Card (PCIe 4.0, 10GB GDDR6X, HDMI 2.1, DisplayPort 1.4a, Dual Ball Fan Bearings, Military-Grade Certification, GPU Tweak II)</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>$ 749</t>
+          <t>$ 638</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -6420,18 +7525,23 @@
       <c r="E223" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>GV-N3080AORUS M-10GD</t>
+          <t>TUF-RTX3080-10G-GAMING-REF</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>$ 749</t>
+          <t>$ 638</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -6447,18 +7557,23 @@
       <c r="E224" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>GIGABYTE AORUS GeForce RTX 3080 Ti 12GB GDDR6X PCI Express 4.0 ATX Video Card GV-N308TAORUS M-12GD</t>
+          <t>GIGABYTE Eagle GeForce RTX 3080 Ti 12GB GDDR6X PCI Express 4.0 ATX Video Card GV-N308TEAGLE OC-12GD</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>$ 799</t>
+          <t>$ 794</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
@@ -6474,18 +7589,23 @@
       <c r="E225" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>GIGABYTE GeForce RTX 3080 VISION OC 10GB Video Card, GV-N3080VISION OC-10GD (REV2.0)</t>
+          <t>GIGABYTE AORUS GeForce RTX 3080 Ti 12GB GDDR6X PCI Express 4.0 ATX Video Card GV-N308TAORUS M-12GD</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>$ 639</t>
+          <t>$ 799</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -6501,18 +7621,23 @@
       <c r="E226" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>GV-N3080VISIONOC-10GDREV2SNRFB</t>
+          <t>GIGABYTE VISION OC GeForce RTX 3080 Ti 12GB GDDR6X PCI Express 4.0 ATX Video Card GV-N308TVISION OC-12GD</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>$ 639</t>
+          <t>$ 779</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -6528,13 +7653,18 @@
       <c r="E227" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>ASUS ROG-STRIX-RTX3080TI-O12G-GAMING ROG STRIX GeForce RTX 3080 Ti Video Card</t>
+          <t>GIGABYTE AORUS GeForce RTX 3080 Ti 12GB GDDR6X PCI Express 4.0 ATX Video Card GV-N308TAORUS M-12GD</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6555,13 +7685,18 @@
       <c r="E228" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F228" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>STRIX-RTX3080TI-O12GSNRFB</t>
+          <t>ASUS ROG-STRIX-RTX3080TI-O12G-GAMING ROG STRIX GeForce RTX 3080 Ti Video Card</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6582,18 +7717,23 @@
       <c r="E229" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F229" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>GIGABYTE VISION OC GeForce RTX 3080 Ti 12GB GDDR6X PCI Express 4.0 ATX Video Card GV-N308TVISION OC-12GD</t>
+          <t>STRIX-RTX3080TI-O12GSNRFB</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>$ 779</t>
+          <t>$ 799</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -6609,18 +7749,23 @@
       <c r="E230" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F230" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>GIGABYTE AORUS GeForce RTX 3080 Ti 12GB GDDR6X PCI Express 4.0 ATX Video Card GV-N308TAORUS M-12GD</t>
+          <t>GIGABYTE Gaming GeForce RTX 3080 Ti 12GB GDDR6X PCI Express 4.0 ATX Video Card GV-N308TGAMING OC-12GD</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>$ 799</t>
+          <t>$ 739</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
@@ -6636,18 +7781,23 @@
       <c r="E231" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F231" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>GIGABYTE Eagle GeForce RTX 3080 Ti 12GB GDDR6X PCI Express 4.0 ATX Video Card GV-N308TEAGLE OC-12GD</t>
+          <t>ASUS ROG STRIX GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 x16 ATX Video Card ROG-STRIX-RTX3080-O10G-WHITE-V2</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>$ 794</t>
+          <t>$ 769</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -6663,13 +7813,18 @@
       <c r="E232" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>ASUS ROG STRIX GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 x16 ATX Video Card ROG-STRIX-RTX3080-O10G-WHITE-V2</t>
+          <t>RTX3080-O10G-WHT-V2</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
@@ -6690,18 +7845,23 @@
       <c r="E233" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>RTX3080-O10G-WHT-V2</t>
+          <t>MSI GeForce RTX 3080 VENTUS 3X 10G 10GB GDDR6X Graphics Card - Black</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>$ 769</t>
+          <t>$ 1,137</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
@@ -6717,18 +7877,23 @@
       <c r="E234" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>GIGABYTE Gaming GeForce RTX 3080 Ti 12GB GDDR6X PCI Express 4.0 ATX Video Card GV-N308TGAMING OC-12GD</t>
+          <t>RTX-3080-VENTUS-3X-10G</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>$ 739</t>
+          <t>$ 1,137</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -6744,18 +7909,23 @@
       <c r="E235" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>ASUS TUF Gaming GeForce RTX 3080 Ti OC Edition Graphics Card(PCIe 4.0,12GB GDDR6X,HDMI 2.1,DisplayPort 1.4a,Dual Ball Fan Bearings,Military-grade Certification),TUF-RTX3080TI-O12G-GAMING</t>
+          <t>GIGABYTE 3080 Graphics card AORUS GIGABYTE GeForce RTX 3080 MASTER 10GB PCI Express 4.0 ATX Video Card (rev. 3.0) GV-N3080AORUS M-10GD (LHR)</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>$ 739</t>
+          <t>$ 749</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
@@ -6771,18 +7941,23 @@
       <c r="E236" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>ASUS TUF Gaming NVIDIA GeForce RTX 3080 Graphics Card (PCIe 4.0, 10GB GDDR6X, HDMI 2.1, DisplayPort 1.4a, Dual Ball Fan Bearings, Military-Grade Certification, GPU Tweak II)</t>
+          <t>GV-N3080AORUS M-10GD</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>$ 638</t>
+          <t>$ 749</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -6798,18 +7973,23 @@
       <c r="E237" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>TUF-RTX3080-10G-GAMING-REF</t>
+          <t>ASUS ROG Strix NVIDIA GeForce RTX 3080 Ti OC Edition Gaming Graphics Card (PCIe 4.0, 12GB GDDR6X, HDMI 2.1) ROG-STRIX-RTX3080TI-O12G-GAMING</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>$ 638</t>
+          <t>$ 799</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
@@ -6825,23 +8005,28 @@
       <c r="E238" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>ASUS ROG Strix GeForce RTX 3080 Video Card ROG-STRIX-RTX3080-O10G-WHITE</t>
+          <t>ROG-STRIX-RTX3080TI-O12G-G</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>$ 879</t>
+          <t>$ 799</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>$7.50 Shipping</t>
+          <t>Free Shipping</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
@@ -6852,23 +8037,28 @@
       <c r="E239" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>STRIXRTX3080O10G-WHT</t>
+          <t>ASUS TUF Gaming GeForce RTX 3080 Ti OC Edition Graphics Card(PCIe 4.0,12GB GDDR6X,HDMI 2.1,DisplayPort 1.4a,Dual Ball Fan Bearings,Military-grade Certification),TUF-RTX3080TI-O12G-GAMING</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>$ 879</t>
+          <t>$ 739</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>$7.50 Shipping</t>
+          <t>Free Shipping</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
@@ -6879,6 +8069,11 @@
       <c r="E240" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
@@ -6908,6 +8103,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F241" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -6935,6 +8135,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -6962,21 +8167,26 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>ASUS ROG Strix NVIDIA GeForce RTX 3080 Ti OC Edition Gaming Graphics Card (PCIe 4.0, 12GB GDDR6X, HDMI 2.1) ROG-STRIX-RTX3080TI-O12G-GAMING</t>
+          <t>ASUS ROG Strix GeForce RTX 3080 Ti OC Edition Gaming Graphics Card (PCIe 4.0, 12GB GDDR6X, HDMI 2.1, DisplayPort 1.4a, Axial-tech Fan Design, 2.9-slot), ROG-STRIX-RTX3080TI-O12G-GAMING</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>$ 799</t>
+          <t>$ 999</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>Free Shipping</t>
+          <t>$6.00 Shipping</t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
@@ -6987,23 +8197,28 @@
       <c r="E244" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>ROG-STRIX-RTX3080TI-O12G-G</t>
+          <t>ROG-STRIX-RTX3080TI-O12G-00</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>$ 799</t>
+          <t>$ 999</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>Free Shipping</t>
+          <t>$6.00 Shipping</t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
@@ -7014,23 +8229,28 @@
       <c r="E245" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F245" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>ASUS ROG STRIX GeForce RTX 3080 Ti Video Card ROG-STRIX-LC-RTX3080TI-O12G-GAMING</t>
+          <t>ASUS ROG Strix GeForce RTX 3080 Video Card ROG-STRIX-RTX3080-O10G-WHITE</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>$ 999</t>
+          <t>$ 879</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>$15.00 Shipping</t>
+          <t>$7.50 Shipping</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
@@ -7041,23 +8261,28 @@
       <c r="E246" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>STX-LC-RTX3080TI-O12</t>
+          <t>STRIXRTX3080O10G-WHT</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>$ 999</t>
+          <t>$ 879</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>$15.00 Shipping</t>
+          <t>$7.50 Shipping</t>
         </is>
       </c>
       <c r="D247" t="inlineStr">
@@ -7068,6 +8293,11 @@
       <c r="E247" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F247" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
@@ -7097,6 +8327,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F248" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -7124,11 +8359,16 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>ASUS ROG Strix GeForce RTX 3080 Ti OC Edition Gaming Graphics Card (PCIe 4.0, 12GB GDDR6X, HDMI 2.1, DisplayPort 1.4a, Axial-tech Fan Design, 2.9-slot), ROG-STRIX-RTX3080TI-O12G-GAMING</t>
+          <t>ASUS ROG STRIX GeForce RTX 3080 Ti Video Card ROG-STRIX-LC-RTX3080TI-O12G-GAMING</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -7138,7 +8378,7 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>$6.00 Shipping</t>
+          <t>$15.00 Shipping</t>
         </is>
       </c>
       <c r="D250" t="inlineStr">
@@ -7149,13 +8389,18 @@
       <c r="E250" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>ROG-STRIX-RTX3080TI-O12G-00</t>
+          <t>STX-LC-RTX3080TI-O12</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -7165,7 +8410,7 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>$6.00 Shipping</t>
+          <t>$15.00 Shipping</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">
@@ -7176,6 +8421,11 @@
       <c r="E251" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>
@@ -7205,6 +8455,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -7232,6 +8487,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -7259,6 +8519,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F254" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -7286,6 +8551,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -7313,6 +8583,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F256" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -7340,6 +8615,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -7367,6 +8647,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -7394,6 +8679,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -7421,6 +8711,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -7448,6 +8743,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -7475,6 +8775,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -7502,6 +8807,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -7529,6 +8839,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F264" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -7556,6 +8871,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F265" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -7583,6 +8903,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -7610,6 +8935,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -7637,6 +8967,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F268" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -7664,6 +8999,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F269" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -7691,6 +9031,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F270" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -7718,6 +9063,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F271" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -7745,6 +9095,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F272" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -7772,6 +9127,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -7799,6 +9159,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F274" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -7826,6 +9191,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -7853,6 +9223,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F276" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -7880,6 +9255,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -7907,6 +9287,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F278" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -7934,6 +9319,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -7961,6 +9351,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -7988,6 +9383,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -8015,6 +9415,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -8042,6 +9447,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -8069,6 +9479,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F284" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -8096,6 +9511,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -8123,6 +9543,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -8150,6 +9575,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -8177,6 +9607,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F288" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
+        </is>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -8202,6 +9637,11 @@
       <c r="E289" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="F289" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/p/pl?d=3080</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add comment and final
</commit_message>
<xml_diff>
--- a/3080.xlsx
+++ b/3080.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G289"/>
+  <dimension ref="A1:F289"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,11 +459,6 @@
           <t>Link of the item</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>features</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -3860,7 +3855,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>GIGABYTE AORUS GeForce RTX 3080 Ti 12GB GDDR6X PCI Express 4.0 ATX Video Card GV-N308TAORUS M-12GD</t>
+          <t>GIGABYTE AORUS GeForce RTX 3080 Ti 12GB GDDR6X PCI Express 4.0 x16 ATX Video Card GV-N308TAORUS M-12GD</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3885,14 +3880,14 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/gigabyte-geforce-rtx-3080-ti-gv-n308taorus-m-12gd/p/N82E16814932539</t>
+          <t>https://www.newegg.com/p/1FT-000A-004W8</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>GIGABYTE AORUS GeForce RTX 3080 Ti 12GB GDDR6X PCI Express 4.0 x16 ATX Video Card GV-N308TAORUS M-12GD</t>
+          <t>GIGABYTE AORUS GeForce RTX 3080 Ti 12GB GDDR6X PCI Express 4.0 ATX Video Card GV-N308TAORUS M-12GD</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3917,7 +3912,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/p/1FT-000A-004W8</t>
+          <t>https://www.newegg.com/gigabyte-geforce-rtx-3080-ti-gv-n308taorus-m-12gd/p/N82E16814932539</t>
         </is>
       </c>
     </row>
@@ -5716,109 +5711,109 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
+          <t>ASUS ROG Strix GeForce RTX 3080 V2 OC Edition 10GB GDDR6X PCI Express 4.0 x16 Video Card ROG-STRIX-RTX3080-O10G-V2-GAMING (LHR)</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>$ 649</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Free Shipping</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>rated 3.3 out of 5</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/asus-geforce-rtx-3080-strix-rtx3080-o10g-v2-gaming/p/1FT-000Y-00971</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>ROG-STRIX-RTX3080-O10G-V2-GAMING</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>$ 649</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Free Shipping</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>rated 3.3 out of 5</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/asus-geforce-rtx-3080-strix-rtx3080-o10g-v2-gaming/p/1FT-000Y-00971</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
           <t>MSI Suprim GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 Video Card RTX 3080 SUPRIM X 10G 
 (LHR)</t>
         </is>
       </c>
-      <c r="B167" t="inlineStr">
+      <c r="B169" t="inlineStr">
         <is>
           <t>$ 678</t>
         </is>
       </c>
-      <c r="C167" t="inlineStr">
-        <is>
-          <t>Free Shipping</t>
-        </is>
-      </c>
-      <c r="D167" t="inlineStr">
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Free Shipping</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
         <is>
           <t>rated 5 out of 5</t>
         </is>
       </c>
-      <c r="E167" t="inlineStr">
+      <c r="E169" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="F167" t="inlineStr">
+      <c r="F169" t="inlineStr">
         <is>
           <t>https://www.newegg.com/msi-geforce-rtx-3080-rtx-3080-suprim-x-10g-lhr/p/1FT-0009-00AS8</t>
-        </is>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>--RTX 3080 SUPRIM X 10G</t>
-        </is>
-      </c>
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>$ 678</t>
-        </is>
-      </c>
-      <c r="C168" t="inlineStr">
-        <is>
-          <t>Free Shipping</t>
-        </is>
-      </c>
-      <c r="D168" t="inlineStr">
-        <is>
-          <t>rated 5 out of 5</t>
-        </is>
-      </c>
-      <c r="E168" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F168" t="inlineStr">
-        <is>
-          <t>https://www.newegg.com/msi-geforce-rtx-3080-rtx-3080-suprim-x-10g-lhr/p/1FT-0009-00AS8</t>
-        </is>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>MSI Gaming GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 ATX Video Card RTX 3080 GAMING Z TRIO 10G LHR</t>
-        </is>
-      </c>
-      <c r="B169" t="inlineStr">
-        <is>
-          <t>$ 619</t>
-        </is>
-      </c>
-      <c r="C169" t="inlineStr">
-        <is>
-          <t>Free Shipping</t>
-        </is>
-      </c>
-      <c r="D169" t="inlineStr">
-        <is>
-          <t>rated 4 out of 5</t>
-        </is>
-      </c>
-      <c r="E169" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F169" t="inlineStr">
-        <is>
-          <t>https://www.newegg.com/p/1FT-0009-008V8</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>RTX 3080 GAMING Z TRIO 10G L</t>
+          <t>--RTX 3080 SUPRIM X 10G</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>$ 619</t>
+          <t>$ 678</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -5828,7 +5823,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>rated 4 out of 5</t>
+          <t>rated 5 out of 5</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
@@ -5838,19 +5833,19 @@
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/p/1FT-0009-008V8</t>
+          <t>https://www.newegg.com/msi-geforce-rtx-3080-rtx-3080-suprim-x-10g-lhr/p/1FT-0009-00AS8</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>MSI Ventus GeForce RTX 3080 Ti 12GB GDDR6X PCI Express 4.0 ATX Video Card -RTX 3080 Ti Ventus 3X 12G OC--</t>
+          <t>MSI Gaming GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 ATX Video Card RTX 3080 GAMING Z TRIO 10G LHR</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>$ 799</t>
+          <t>$ 619</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -5870,19 +5865,19 @@
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/msi-geforce-rtx-3080-ti-rtx-3080-ti-ventus-3x-12g-oc/p/1FT-0009-00AW2</t>
+          <t>https://www.newegg.com/p/1FT-0009-008V8</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>-RTX 3080 Ti Ventus 3X</t>
+          <t>RTX 3080 GAMING Z TRIO 10G L</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>$ 799</t>
+          <t>$ 619</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -5902,19 +5897,19 @@
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/msi-geforce-rtx-3080-ti-rtx-3080-ti-ventus-3x-12g-oc/p/1FT-0009-00AW2</t>
+          <t>https://www.newegg.com/p/1FT-0009-008V8</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>ASUS ROG Strix GeForce RTX 3080 V2 OC Edition 10GB GDDR6X PCI Express 4.0 x16 Video Card ROG-STRIX-RTX3080-O10G-V2-GAMING (LHR)</t>
+          <t>MSI Ventus GeForce RTX 3080 Ti 12GB GDDR6X PCI Express 4.0 ATX Video Card -RTX 3080 Ti Ventus 3X 12G OC--</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>$ 649</t>
+          <t>$ 799</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -5934,19 +5929,19 @@
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/asus-geforce-rtx-3080-strix-rtx3080-o10g-v2-gaming/p/1FT-000Y-00971</t>
+          <t>https://www.newegg.com/msi-geforce-rtx-3080-ti-rtx-3080-ti-ventus-3x-12g-oc/p/1FT-0009-00AW2</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>ROG-STRIX-RTX3080-O10G-V2-GAMING</t>
+          <t>-RTX 3080 Ti Ventus 3X</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>$ 649</t>
+          <t>$ 799</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -5966,7 +5961,7 @@
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/asus-geforce-rtx-3080-strix-rtx3080-o10g-v2-gaming/p/1FT-000Y-00971</t>
+          <t>https://www.newegg.com/msi-geforce-rtx-3080-ti-rtx-3080-ti-ventus-3x-12g-oc/p/1FT-0009-00AW2</t>
         </is>
       </c>
     </row>
@@ -6293,12 +6288,12 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>MSI Gaming GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 Video Card RTX 3080 GAMING X TRIO 10G</t>
+          <t>MSI RTX 3080 SUPRIM X 10G LHR Suprim GeForce RTX 3080 Video Card</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>$ 619</t>
+          <t>$ 678</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -6318,19 +6313,19 @@
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/p/1FT-0009-00BH5</t>
+          <t>https://www.newegg.com/msi-geforce-rtx-3080-rtx-3080-suprim-x-10g-lhr/p/1FT-0009-009K4</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>RTX 3080 GAMING X TRIO 10</t>
+          <t>RTX3080SuprimX10GLHRSNRFB</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>$ 619</t>
+          <t>$ 678</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -6350,19 +6345,19 @@
       </c>
       <c r="F186" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/p/1FT-0009-00BH5</t>
+          <t>https://www.newegg.com/msi-geforce-rtx-3080-rtx-3080-suprim-x-10g-lhr/p/1FT-0009-009K4</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>MSI RTX 3080 SUPRIM X 10G LHR Suprim GeForce RTX 3080 Video Card</t>
+          <t>GIGABYTE Gaming OC GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 ATX Video Card GV-N3080GAMING OC-10GD (rev. 2.0) (LHR)</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>$ 678</t>
+          <t>$ 679</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -6382,19 +6377,19 @@
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/msi-geforce-rtx-3080-rtx-3080-suprim-x-10g-lhr/p/1FT-0009-009K4</t>
+          <t>https://www.newegg.com/p/1FT-000A-006E0</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>RTX3080SuprimX10GLHRSNRFB</t>
+          <t>GV-N3080GAMING OC-10GD REV</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>$ 678</t>
+          <t>$ 679</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -6414,24 +6409,24 @@
       </c>
       <c r="F188" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/msi-geforce-rtx-3080-rtx-3080-suprim-x-10g-lhr/p/1FT-0009-009K4</t>
+          <t>https://www.newegg.com/p/1FT-000A-006E0</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>GIGABYTE Gaming OC GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 ATX Video Card GV-N3080GAMING OC-10GD (rev. 2.0) (LHR)</t>
+          <t>MSI GeForce RTX 3080 Suprim X 10G LHR 10GB GDRR6X 320-Bit HDMI/DP Graphics Card</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>$ 679</t>
+          <t>$ 699</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>Free Shipping</t>
+          <t>$7.00 Shipping</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
@@ -6446,24 +6441,24 @@
       </c>
       <c r="F189" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/p/1FT-000A-006E0</t>
+          <t>https://www.newegg.com/msi-rtx3080suprimx10glhr/p/1FT-0009-006M1</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>GV-N3080GAMING OC-10GD REV</t>
+          <t>RTX3080SUPRIMX10GLHR</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>$ 679</t>
+          <t>$ 699</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>Free Shipping</t>
+          <t>$7.00 Shipping</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
@@ -6478,24 +6473,24 @@
       </c>
       <c r="F190" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/p/1FT-000A-006E0</t>
+          <t>https://www.newegg.com/msi-rtx3080suprimx10glhr/p/1FT-0009-006M1</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>MSI GeForce RTX 3080 Suprim X 10G LHR 10GB GDRR6X 320-Bit HDMI/DP Graphics Card</t>
+          <t>GIGABYTE Gaming GeForce RTX 3080 Ti Video Card GV-N308TGAMING OC-12GD</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>$ 699</t>
+          <t>$ 959</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>$7.00 Shipping</t>
+          <t>Free Shipping</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
@@ -6510,24 +6505,24 @@
       </c>
       <c r="F191" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/msi-rtx3080suprimx10glhr/p/1FT-0009-006M1</t>
+          <t>https://www.newegg.com/gigabyte-geforce-rtx-3080-ti-gv-n308tgaming-oc-12gd/p/1FT-000A-006D3</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>RTX3080SUPRIMX10GLHR</t>
+          <t>MSI Gaming GeForce RTX 3080 10GB GDDR6X PCI Express 4.0 Video Card RTX 3080 GAMING X TRIO 10G</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>$ 699</t>
+          <t>$ 619</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>$7.00 Shipping</t>
+          <t>Free Shipping</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
@@ -6542,19 +6537,19 @@
       </c>
       <c r="F192" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/msi-rtx3080suprimx10glhr/p/1FT-0009-006M1</t>
+          <t>https://www.newegg.com/p/1FT-0009-00BH5</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>GIGABYTE Gaming GeForce RTX 3080 Ti Video Card GV-N308TGAMING OC-12GD</t>
+          <t>RTX 3080 GAMING X TRIO 10</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>$ 959</t>
+          <t>$ 619</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -6574,7 +6569,7 @@
       </c>
       <c r="F193" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/gigabyte-geforce-rtx-3080-ti-gv-n308tgaming-oc-12gd/p/1FT-000A-006D3</t>
+          <t>https://www.newegg.com/p/1FT-0009-00BH5</t>
         </is>
       </c>
     </row>
@@ -9557,12 +9552,12 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>EVGA GeForce RTX 3080 Ti XC3 ULTRA 12GB GDDR6X LHR Graphics Card 12G-P5-3955-KR</t>
+          <t>EVGA GeForce RTX 3080 FTW3 ULTRA GAMING Video Card, 10G-P5-3897-KL, 10GB GDDR6X, iCX3 Technology, ARGB LED, Metal Backplate, LHR</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>$ 1,099</t>
+          <t>$ 885</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -9582,19 +9577,19 @@
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/evga-12g-p5-3955-kr/p/1FT-001K-00DY1</t>
+          <t>https://www.newegg.com/evga-10g-p5-3897-kl/p/1FT-001K-00DF7</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>EVGA GeForce RTX 3080 FTW3 ULTRA GAMING Video Card, 10G-P5-3897-KL, 10GB GDDR6X, iCX3 Technology, ARGB LED, Metal Backplate, LHR</t>
+          <t>EVGA GeForce RTX 3080 Ti XC3 ULTRA 12GB GDDR6X LHR Graphics Card 12G-P5-3955-KR</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>$ 885</t>
+          <t>$ 1,099</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -9614,7 +9609,7 @@
       </c>
       <c r="F288" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/evga-10g-p5-3897-kl/p/1FT-001K-00DF7</t>
+          <t>https://www.newegg.com/evga-12g-p5-3955-kr/p/1FT-001K-00DY1</t>
         </is>
       </c>
     </row>

</xml_diff>